<commit_message>
Copy encounters from GM Binder into sheets
</commit_message>
<xml_diff>
--- a/RandomEncounterTableBuilder.xlsx
+++ b/RandomEncounterTableBuilder.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanks\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A27B02E-4713-4E11-9D65-377CF461AC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777C5018-BBCC-46E8-BFD4-BFFDB12DA4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{541EB1F5-CB9A-4BF1-8008-7EE9CFB174A5}"/>
   </bookViews>
   <sheets>
-    <sheet name="HowlingRidge" sheetId="1" r:id="rId1"/>
+    <sheet name="TitanGripMountains" sheetId="5" r:id="rId1"/>
+    <sheet name="TheAshenCrags" sheetId="4" r:id="rId2"/>
+    <sheet name="XiocoatlPeaks" sheetId="3" r:id="rId3"/>
+    <sheet name="HowlingRidge" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="125">
   <si>
     <t>Percentage</t>
   </si>
@@ -170,7 +173,244 @@
     <t>A memorial site dedicated to the memory of travelers who've perished here</t>
   </si>
   <si>
+    <t>Size 3 Falling Debris</t>
+  </si>
+  <si>
     <t>Copy Into Doc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Small Fall Hidden by Fog (DC 15 to Spot) </t>
+  </si>
+  <si>
+    <t>A Medium Fall Hidden by Fog (DC 15 to Spot)</t>
+  </si>
+  <si>
+    <t>2d6 **skink cohorts** + 1d6 **skink skirmishers**</t>
+  </si>
+  <si>
+    <t>1 **skink chieftain** + 2d4 **skink cohorts** + 1d4 **skink skirmishers**</t>
+  </si>
+  <si>
+    <t>2d4 **saurus warriors**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 **saurus warriors** (with the Blessing of the Beast God) riding **cold ones** </t>
+  </si>
+  <si>
+    <t>1d4 **saurus warriors** + 2d4 **skink skirmishers**</t>
+  </si>
+  <si>
+    <t>1d6 + 1 **cold ones**</t>
+  </si>
+  <si>
+    <t>2d12 **chimpanzees**</t>
+  </si>
+  <si>
+    <t>2d4 **gorillas**</t>
+  </si>
+  <si>
+    <t>1d6 **gorillas** + 2d6 **chimpanzees**</t>
+  </si>
+  <si>
+    <t>1 **giant ape** + 1d4 + 1 **chimpanzees**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 **giant apes** </t>
+  </si>
+  <si>
+    <t>2d10 **condors** feeding on the remains left by an ape vs. lizardmen battle</t>
+  </si>
+  <si>
+    <t>2d8 **agentavis** feeding on the remains left by an ape vs. lizardmen battle</t>
+  </si>
+  <si>
+    <t>2d6 **dread agentavis** feeding on the remains left by an ape vs. lizardmen battle</t>
+  </si>
+  <si>
+    <t>A random encounter of lizardmen battling a random encounter of apes</t>
+  </si>
+  <si>
+    <t>Treasure hunters (2d6 + 2 **bandits**) hoping to plunders some of the ruins</t>
+  </si>
+  <si>
+    <t>A **skink skirmisher** offering to aid the players if they help it repel an ape attack against one of their holdings</t>
+  </si>
+  <si>
+    <t>A **gorilla** trying to lead the players back to its nest so they can aid its troop in fighting off an incoming wave of lizardmen</t>
+  </si>
+  <si>
+    <t>A river leading into a mountain pond</t>
+  </si>
+  <si>
+    <t>An ancient ruin occupied by apes or lizardmen</t>
+  </si>
+  <si>
+    <t>1d4 **swarms of poisonous snakes**</t>
+  </si>
+  <si>
+    <t>2d8 **giant poisonous snakes**</t>
+  </si>
+  <si>
+    <t>1d3 **giant constrictor snakes**</t>
+  </si>
+  <si>
+    <t>The **titanic ape** leading an assault against a lizardman temple</t>
+  </si>
+  <si>
+    <t>An overgrown ruin carved into the mountainside with unknown occupants</t>
+  </si>
+  <si>
+    <t>Size 3 Rockslide</t>
+  </si>
+  <si>
+    <t>Size 4 Rockslide</t>
+  </si>
+  <si>
+    <t>Size 4 Falling Debris</t>
+  </si>
+  <si>
+    <t>A Small Fall Hidden by Ash Clouds (DC 15 to Spot)</t>
+  </si>
+  <si>
+    <t>A Medium Fall Hidden by Ash Clouds (DC 15 to Spot)</t>
+  </si>
+  <si>
+    <t>Chaos dwarf wreckage from a supply train or destroyed machinery.</t>
+  </si>
+  <si>
+    <t>1d10 **fire elementals**</t>
+  </si>
+  <si>
+    <t>An Expeditionary Force of 1d6 + 1 **chaos dwarf blazing beard warriors** and 1d6 + 1 **chaos dwarf blunderbussiers**</t>
+  </si>
+  <si>
+    <t>An Elite Expeditionary Force of 1d4 + 1 **chaos dwarf infernal guard, axemen** and 1d4 + 1 **chaos dwarf infernal guard, fireglaivadiers**</t>
+  </si>
+  <si>
+    <t>A squad of 1d8 + 1 **chaos dwarf infernal ironsworn**</t>
+  </si>
+  <si>
+    <t>2d4 **hell hounds**</t>
+  </si>
+  <si>
+    <t>1 renegade **infernal destroyer**</t>
+  </si>
+  <si>
+    <t>1 **iron golem**</t>
+  </si>
+  <si>
+    <t>1d4 **soul grinders**</t>
+  </si>
+  <si>
+    <t>1 **daemon prince** with the wings enhancement accompanied by a flock of 3d4 **chaos furies**</t>
+  </si>
+  <si>
+    <t>A gnomish explorer (**spy**), hoping to study and salvage abandoned machinery.</t>
+  </si>
+  <si>
+    <t>A rag-tag community of escaped laborers eeking out a life among the ruins of a chaos dwarf outpost.</t>
+  </si>
+  <si>
+    <t>A random encounter of chaos dwarves battling one of the other random creature encounters for control of a dwarven outpost.</t>
+  </si>
+  <si>
+    <t>An expedition of mountain dwarves (2d6 + 2 **veterans** and 3d8 + 5 **guards**) looking to demolish any remaining chaos dwarf holds to prevent them from falling back into enemy hands.</t>
+  </si>
+  <si>
+    <t>The abandoned remains of a chaos dwarf hold.</t>
+  </si>
+  <si>
+    <t>A chaos dwarf hold which has been recaptured by chaos dwarves.</t>
+  </si>
+  <si>
+    <t>A chaos dwarf hold which has been captured by a daemon prince leading a small fiendish army.</t>
+  </si>
+  <si>
+    <t>Size 3 Avalanche or Rockslide</t>
+  </si>
+  <si>
+    <t>Size 4 Avalanche or Rockslide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size 3 Falling Debris </t>
+  </si>
+  <si>
+    <t>A Small Fall Hidden by Fog or Snow (DC 15 to Spot)</t>
+  </si>
+  <si>
+    <t>A Medium Fall Hidden by Fog or Snow (DC 15 to Spot)</t>
+  </si>
+  <si>
+    <t>A Large Fall Hidden by Fog or Snow (DC 15 to Spot)</t>
+  </si>
+  <si>
+    <t>1d4 + 1 **dzu-teh yetis** leading 2d8 **teh-lma yetis**</t>
+  </si>
+  <si>
+    <t>1d4 + 1 **meh-teh yetis** leading 2d8 **teh-lma yetis**</t>
+  </si>
+  <si>
+    <t>2d10 **yeti stalkers**</t>
+  </si>
+  <si>
+    <t>1d4 **abominable yetis** with 2d4 + 2 **yetis**</t>
+  </si>
+  <si>
+    <t>1 **zheng mountain breaker** leading 1d4 + 1 **zheng**</t>
+  </si>
+  <si>
+    <t>1 **zheng summit sovereign** atop a mountain peak ruling over 2d4 + 2 **zheng**</t>
+  </si>
+  <si>
+    <t>1d4 **adult white dragons**</t>
+  </si>
+  <si>
+    <t>1d4 **remorhaz**</t>
+  </si>
+  <si>
+    <t>2d6 + 1 **frost giants**</t>
+  </si>
+  <si>
+    <t>2d4 + 1 **cloud giants**</t>
+  </si>
+  <si>
+    <t>1d3 **storm giants**</t>
+  </si>
+  <si>
+    <t>An **ancient white dragon** seeking out a new lair</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An **empyrean** ruling over a divine mountain peak</t>
+  </si>
+  <si>
+    <t>An expedition of mountaineers (3d8 + 5 **veterans** and 3d6 + 3 **scouts**) looking to recover lost giant artifacts.</t>
+  </si>
+  <si>
+    <t>A monastery of monks under the guidance of a **meh-teh yeti**</t>
+  </si>
+  <si>
+    <t>A brutal warlord **ADD STAT BLOCKs** leading a tribe of warriors as they attempt to coerce a group a savage yetis to join them in war.</t>
+  </si>
+  <si>
+    <t>A yeti burial ground at the bottom of a deep crevasse.</t>
+  </si>
+  <si>
+    <t>2d10 **terror goats**</t>
+  </si>
+  <si>
+    <t>A battle between the meh-teh encounter and another yeti encounter</t>
+  </si>
+  <si>
+    <t>A battle between a yeti encounter and a giant encounter</t>
+  </si>
+  <si>
+    <t>Seemingly unoccupied giant ruins</t>
+  </si>
+  <si>
+    <t>Giant ruins occupied by yetis</t>
+  </si>
+  <si>
+    <t>Giant ruins being reclaimed by giants</t>
   </si>
 </sst>
 </file>
@@ -584,12 +824,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9C6F01-5ACC-4DF7-9964-D17E91C7E36A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C890DE-A4B7-47C7-BE9B-9A2FF2177ABA}">
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -668,39 +908,39 @@
         <v>41</v>
       </c>
       <c r="G2" s="4">
-        <f>SUMIF($B$4:$B$31, G1,$C$4:$C$31)</f>
+        <f>SUMIF($B$4:$B31, G1,$C$4:$C31)</f>
         <v>15</v>
       </c>
       <c r="H2" s="4">
-        <f>SUMIF($B$4:$B$31, H1,$C$4:$C$31)</f>
+        <f>SUMIF($B$4:$B31, H1,$C$4:$C31)</f>
         <v>16</v>
       </c>
       <c r="I2" s="4">
-        <f>SUMIF($B$4:$B$31, I1,$C$4:$C$31)</f>
+        <f>SUMIF($B$4:$B31, I1,$C$4:$C31)</f>
         <v>20</v>
       </c>
       <c r="J2" s="4">
-        <f>SUMIF($B$4:$B$31, J1,$C$4:$C$31)</f>
+        <f>SUMIF($B$4:$B31, J1,$C$4:$C31)</f>
         <v>18</v>
       </c>
       <c r="K2" s="4">
-        <f>SUMIF($B$4:$B$31, K1,$C$4:$C$31)</f>
+        <f>SUMIF($B$4:$B31, K1,$C$4:$C31)</f>
         <v>6</v>
       </c>
       <c r="L2" s="4">
-        <f>SUMIF($B$4:$B$31, L1,$C$4:$C$31)</f>
-        <v>8</v>
+        <f>SUMIF($B$4:$B31, L1,$C$4:$C31)</f>
+        <v>6</v>
       </c>
       <c r="M2" s="4">
-        <f>SUMIF($B$4:$B$31, M1,$C$4:$C$31)</f>
-        <v>4</v>
+        <f>SUMIF($B$4:$B31, M1,$C$4:$C31)</f>
+        <v>6</v>
       </c>
       <c r="N2" s="4">
-        <f>SUMIF($B$4:$B$31, N1,$C$4:$C$31)</f>
+        <f>SUMIF($B$4:$B31, N1,$C$4:$C31)</f>
         <v>11</v>
       </c>
       <c r="O2" s="4">
-        <f>SUMIF($B$4:$B$31, O1,$C$4:$C$31)</f>
+        <f>SUMIF($B$4:$B31, O1,$C$4:$C31)</f>
         <v>2</v>
       </c>
       <c r="P2" s="4">
@@ -715,7 +955,2401 @@
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4+(C4-1)</f>
+        <v>3</v>
+      </c>
+      <c r="F4" t="str">
+        <f>"|" &amp; D4 &amp; "-" &amp; E4 &amp; "|" &amp; A4 &amp; "|"</f>
+        <v>|1-3|Size 3 Avalanche or Rockslide|</v>
+      </c>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <f>E4+1</f>
+        <v>4</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" ref="E5:E31" si="0">D5+(C5-1)</f>
+        <v>5</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" ref="F5:F31" si="1">"|" &amp; D5 &amp; "-" &amp; E5 &amp; "|" &amp; A5 &amp; "|"</f>
+        <v>|4-5|Size 4 Avalanche or Rockslide|</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ref="D6:D33" si="2">E5+1</f>
+        <v>6</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>|6-7|Size 3 Falling Debris |</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>|8-10|Size 4 Falling Debris|</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>|11-13|A Small Fall Hidden by Fog or Snow (DC 15 to Spot)|</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>|14-15|A Medium Fall Hidden by Fog or Snow (DC 15 to Spot)|</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="3">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>|16-19|A Large Fall Hidden by Fog or Snow (DC 15 to Spot)|</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>|20-23|1d4 + 1 **dzu-teh yetis** leading 2d8 **teh-lma yetis**|</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="1"/>
+        <v>|24-27|1d4 + 1 **meh-teh yetis** leading 2d8 **teh-lma yetis**|</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>|28-31|2d10 **yeti stalkers**|</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>|32-36|1d4 **abominable yetis** with 2d4 + 2 **yetis**|</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="3">
+        <v>5</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>|37-41|1 **zheng mountain breaker** leading 1d4 + 1 **zheng**|</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3">
+        <v>5</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>|42-46|1 **zheng summit sovereign** atop a mountain peak ruling over 2d4 + 2 **zheng**|</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="3">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>|47-51|1d4 **adult white dragons**|</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="3">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>|52-57|1d4 **remorhaz**|</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="3">
+        <v>6</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v>|58-63|2d6 + 1 **frost giants**|</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="3">
+        <v>6</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
+        <v>|64-69|2d4 + 1 **cloud giants**|</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="3">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
+        <v>|70-75|1d3 **storm giants**|</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="1"/>
+        <v>|76-77|An **ancient white dragon** seeking out a new lair|</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="1"/>
+        <v>|78-79| An **empyrean** ruling over a divine mountain peak|</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="1"/>
+        <v>|80-81|An expedition of mountaineers (3d8 + 5 **veterans** and 3d6 + 3 **scouts**) looking to recover lost giant artifacts.|</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="1"/>
+        <v>|82-83|A monastery of monks under the guidance of a **meh-teh yeti**|</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="1"/>
+        <v>|84-85|A brutal warlord **ADD STAT BLOCKs** leading a tribe of warriors as they attempt to coerce a group a savage yetis to join them in war.|</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="1"/>
+        <v>|86-88|A yeti burial ground at the bottom of a deep crevasse.|</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="3">
+        <v>3</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="1"/>
+        <v>|89-91|2d10 **terror goats**|</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="3">
+        <v>5</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="1"/>
+        <v>|92-96|A battle between the meh-teh encounter and another yeti encounter|</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="2"/>
+        <v>97</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="1"/>
+        <v>|97-98|A battle between a yeti encounter and a giant encounter|</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="1"/>
+        <v>|99-100|Seemingly unoccupied giant ruins|</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="3">
+        <v>3</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" ref="E32:E33" si="3">D32+(C32-1)</f>
+        <v>103</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" ref="F32:F33" si="4">"|" &amp; D32 &amp; "-" &amp; E32 &amp; "|" &amp; A32 &amp; "|"</f>
+        <v>|101-103|Giant ruins occupied by yetis|</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="3">
+        <v>4</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="3"/>
+        <v>107</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="4"/>
+        <v>|104-107|Giant ruins being reclaimed by giants|</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="6"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17ED0843-FA45-481F-ADB0-D654576F0FEF}">
+  <dimension ref="A1:P35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="4">
+        <f>SUMIF($B$4:$B31, G1,$C$4:$C31)</f>
+        <v>15</v>
+      </c>
+      <c r="H2" s="4">
+        <f>SUMIF($B$4:$B31, H1,$C$4:$C31)</f>
+        <v>16</v>
+      </c>
+      <c r="I2" s="4">
+        <f>SUMIF($B$4:$B31, I1,$C$4:$C31)</f>
+        <v>20</v>
+      </c>
+      <c r="J2" s="4">
+        <f>SUMIF($B$4:$B31, J1,$C$4:$C31)</f>
+        <v>18</v>
+      </c>
+      <c r="K2" s="4">
+        <f>SUMIF($B$4:$B31, K1,$C$4:$C31)</f>
+        <v>6</v>
+      </c>
+      <c r="L2" s="4">
+        <f>SUMIF($B$4:$B31, L1,$C$4:$C31)</f>
+        <v>8</v>
+      </c>
+      <c r="M2" s="4">
+        <f>SUMIF($B$4:$B31, M1,$C$4:$C31)</f>
+        <v>2</v>
+      </c>
+      <c r="N2" s="4">
+        <f>SUMIF($B$4:$B31, N1,$C$4:$C31)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="4">
+        <f>SUMIF($B$4:$B31, O1,$C$4:$C31)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="4">
+        <f>SUM(G2:O2)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4+(C4-1)</f>
+        <v>3</v>
+      </c>
+      <c r="F4" t="str">
+        <f>"|" &amp; D4 &amp; "-" &amp; E4 &amp; "|" &amp; A4 &amp; "|"</f>
+        <v>|1-3|Size 3 Rockslide|</v>
+      </c>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <f>E4+1</f>
+        <v>4</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" ref="E5:E31" si="0">D5+(C5-1)</f>
+        <v>5</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" ref="F5:F31" si="1">"|" &amp; D5 &amp; "-" &amp; E5 &amp; "|" &amp; A5 &amp; "|"</f>
+        <v>|4-5|Size 4 Rockslide|</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ref="D6:D31" si="2">E5+1</f>
+        <v>6</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>|6-7|Size 3 Falling Debris|</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>|8-10|Size 4 Falling Debris|</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>|11-13|A Small Fall Hidden by Ash Clouds (DC 15 to Spot)|</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>|14-15|A Medium Fall Hidden by Ash Clouds (DC 15 to Spot)|</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="3">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>|16-19|Chaos dwarf wreckage from a supply train or destroyed machinery.|</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>|20-23|1d10 **fire elementals**|</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="1"/>
+        <v>|24-27|An Expeditionary Force of 1d6 + 1 **chaos dwarf blazing beard warriors** and 1d6 + 1 **chaos dwarf blunderbussiers**|</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>|28-31|An Elite Expeditionary Force of 1d4 + 1 **chaos dwarf infernal guard, axemen** and 1d4 + 1 **chaos dwarf infernal guard, fireglaivadiers**|</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>|32-36|A squad of 1d8 + 1 **chaos dwarf infernal ironsworn**|</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="3">
+        <v>5</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>|37-41|2d4 **hell hounds**|</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3">
+        <v>5</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>|42-46|1 renegade **infernal destroyer**|</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="3">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>|47-51|1 **iron golem**|</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="3">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>|52-57|1d4 **soul grinders**|</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="3">
+        <v>6</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v>|58-63|1 **daemon prince** with the wings enhancement accompanied by a flock of 3d4 **chaos furies**|</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="3">
+        <v>6</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
+        <v>|64-69|A gnomish explorer (**spy**), hoping to study and salvage abandoned machinery.|</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="3">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
+        <v>|70-75|A rag-tag community of escaped laborers eeking out a life among the ruins of a chaos dwarf outpost.|</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="1"/>
+        <v>|76-77|A random encounter of chaos dwarves battling one of the other random creature encounters for control of a dwarven outpost.|</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="1"/>
+        <v>|78-79|An expedition of mountain dwarves (2d6 + 2 **veterans** and 3d8 + 5 **guards**) looking to demolish any remaining chaos dwarf holds to prevent them from falling back into enemy hands.|</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="1"/>
+        <v>|80-81|The abandoned remains of a chaos dwarf hold.|</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="1"/>
+        <v>|82-83|A chaos dwarf hold which has been recaptured by chaos dwarves.|</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="1"/>
+        <v>|84-85|A chaos dwarf hold which has been captured by a daemon prince leading a small fiendish army.|</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E786A9-CB1A-44D9-97AD-FFFFA23AECE7}">
+  <dimension ref="A1:P35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="4">
+        <f>SUMIF($B$4:$B32, G1,$C$4:$C32)</f>
+        <v>15</v>
+      </c>
+      <c r="H2" s="4">
+        <f>SUMIF($B$4:$B32, H1,$C$4:$C32)</f>
+        <v>16</v>
+      </c>
+      <c r="I2" s="4">
+        <f>SUMIF($B$4:$B32, I1,$C$4:$C32)</f>
+        <v>20</v>
+      </c>
+      <c r="J2" s="4">
+        <f>SUMIF($B$4:$B32, J1,$C$4:$C32)</f>
+        <v>18</v>
+      </c>
+      <c r="K2" s="4">
+        <f>SUMIF($B$4:$B32, K1,$C$4:$C32)</f>
+        <v>6</v>
+      </c>
+      <c r="L2" s="4">
+        <f>SUMIF($B$4:$B32, L1,$C$4:$C32)</f>
+        <v>8</v>
+      </c>
+      <c r="M2" s="4">
+        <f>SUMIF($B$4:$B32, M1,$C$4:$C32)</f>
+        <v>4</v>
+      </c>
+      <c r="N2" s="4">
+        <f>SUMIF($B$4:$B32, N1,$C$4:$C32)</f>
+        <v>11</v>
+      </c>
+      <c r="O2" s="4">
+        <f>SUMIF($B$4:$B32, O1,$C$4:$C32)</f>
+        <v>4</v>
+      </c>
+      <c r="P2" s="4">
+        <f>SUM(G2:O2)</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4+(C4-1)</f>
+        <v>3</v>
+      </c>
+      <c r="F4" t="str">
+        <f>"|" &amp; D4 &amp; "-" &amp; E4 &amp; "|" &amp; A4 &amp; "|"</f>
+        <v>|1-3|Size 2 Falling Debris|</v>
+      </c>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <f>E4+1</f>
+        <v>4</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" ref="E5:E31" si="0">D5+(C5-1)</f>
+        <v>5</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" ref="F5:F31" si="1">"|" &amp; D5 &amp; "-" &amp; E5 &amp; "|" &amp; A5 &amp; "|"</f>
+        <v>|4-5|Size 3 Falling Debris|</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ref="D6:D32" si="2">E5+1</f>
+        <v>6</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>|6-7|A Small Fall Hidden by Fog (DC 15 to Spot) |</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>|8-10|A Medium Fall Hidden by Fog (DC 15 to Spot)|</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>|11-13|2d6 **skink cohorts** + 1d6 **skink skirmishers**|</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>|14-15|1 **skink chieftain** + 2d4 **skink cohorts** + 1d4 **skink skirmishers**|</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="3">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>|16-19|2d4 **saurus warriors**|</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>|20-23|2 **saurus warriors** (with the Blessing of the Beast God) riding **cold ones** |</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="1"/>
+        <v>|24-27|1d4 **saurus warriors** + 2d4 **skink skirmishers**|</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>|28-31|1d6 + 1 **cold ones**|</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>|32-36|2d12 **chimpanzees**|</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="3">
+        <v>5</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>|37-41|2d4 **gorillas**|</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3">
+        <v>5</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>|42-46|1d6 **gorillas** + 2d6 **chimpanzees**|</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="3">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>|47-51|1 **giant ape** + 1d4 + 1 **chimpanzees**|</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="3">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>|52-57|2 **giant apes** |</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="3">
+        <v>6</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v>|58-63|2d10 **condors** feeding on the remains left by an ape vs. lizardmen battle|</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="3">
+        <v>6</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
+        <v>|64-69|2d8 **agentavis** feeding on the remains left by an ape vs. lizardmen battle|</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="3">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
+        <v>|70-75|2d6 **dread agentavis** feeding on the remains left by an ape vs. lizardmen battle|</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="1"/>
+        <v>|76-77|A random encounter of lizardmen battling a random encounter of apes|</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="1"/>
+        <v>|78-79|Treasure hunters (2d6 + 2 **bandits**) hoping to plunders some of the ruins|</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="1"/>
+        <v>|80-81|A **skink skirmisher** offering to aid the players if they help it repel an ape attack against one of their holdings|</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="1"/>
+        <v>|82-83|A **gorilla** trying to lead the players back to its nest so they can aid its troop in fighting off an incoming wave of lizardmen|</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="1"/>
+        <v>|84-85|A river leading into a mountain pond|</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="1"/>
+        <v>|86-88|An ancient ruin occupied by apes or lizardmen|</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="3">
+        <v>3</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="1"/>
+        <v>|89-91|1d4 **swarms of poisonous snakes**|</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="3">
+        <v>5</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="1"/>
+        <v>|92-96|2d8 **giant poisonous snakes**|</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="2"/>
+        <v>97</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="1"/>
+        <v>|97-98|1d3 **giant constrictor snakes**|</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="1"/>
+        <v>|99-100|The **titanic ape** leading an assault against a lizardman temple|</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" ref="E32" si="3">D32+(C32-1)</f>
+        <v>102</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" ref="F32" si="4">"|" &amp; D32 &amp; "-" &amp; E32 &amp; "|" &amp; A32 &amp; "|"</f>
+        <v>|101-102|An overgrown ruin carved into the mountainside with unknown occupants|</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9C6F01-5ACC-4DF7-9964-D17E91C7E36A}">
+  <dimension ref="A1:P35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="4">
+        <f>SUMIF($B$4:$B31, G1,$C$4:$C31)</f>
+        <v>15</v>
+      </c>
+      <c r="H2" s="4">
+        <f>SUMIF($B$4:$B31, H1,$C$4:$C31)</f>
+        <v>16</v>
+      </c>
+      <c r="I2" s="4">
+        <f>SUMIF($B$4:$B31, I1,$C$4:$C31)</f>
+        <v>20</v>
+      </c>
+      <c r="J2" s="4">
+        <f>SUMIF($B$4:$B31, J1,$C$4:$C31)</f>
+        <v>18</v>
+      </c>
+      <c r="K2" s="4">
+        <f>SUMIF($B$4:$B31, K1,$C$4:$C31)</f>
+        <v>6</v>
+      </c>
+      <c r="L2" s="4">
+        <f>SUMIF($B$4:$B31, L1,$C$4:$C31)</f>
+        <v>8</v>
+      </c>
+      <c r="M2" s="4">
+        <f>SUMIF($B$4:$B31, M1,$C$4:$C31)</f>
+        <v>4</v>
+      </c>
+      <c r="N2" s="4">
+        <f>SUMIF($B$4:$B31, N1,$C$4:$C31)</f>
+        <v>11</v>
+      </c>
+      <c r="O2" s="4">
+        <f>SUMIF($B$4:$B31, O1,$C$4:$C31)</f>
+        <v>2</v>
+      </c>
+      <c r="P2" s="4">
+        <f>SUM(G2:O2)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>

</xml_diff>